<commit_message>
complete loainhanvien & khachhang
</commit_message>
<xml_diff>
--- a/process.xlsx
+++ b/process.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
   <si>
     <t xml:space="preserve">Tuần </t>
   </si>
@@ -191,11 +191,13 @@
     <t>Bảo 30%, Nam 70%</t>
   </si>
   <si>
-    <t>còn form KH thảo luận
-cần thảo luận với bạn</t>
-  </si>
-  <si>
     <t>Đang thực hiện</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chưa làm kịp </t>
+  </si>
+  <si>
+    <t>hoàn thành</t>
   </si>
 </sst>
 </file>
@@ -571,6 +573,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -603,9 +608,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -960,7 +962,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -975,14 +977,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="1:6" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -995,37 +997,37 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="36" t="s">
+      <c r="E3" s="33"/>
+      <c r="F3" s="37" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="37"/>
+      <c r="F4" s="38"/>
     </row>
     <row r="5" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27">
+      <c r="A5" s="28">
         <v>1</v>
       </c>
       <c r="B5" s="25" t="s">
@@ -1045,7 +1047,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="18" t="s">
         <v>10</v>
       </c>
@@ -1063,7 +1065,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="18" t="s">
         <v>11</v>
       </c>
@@ -1081,7 +1083,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="19" t="s">
         <v>12</v>
       </c>
@@ -1099,7 +1101,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
+      <c r="A9" s="29">
         <v>2</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -1119,7 +1121,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="18" t="s">
         <v>14</v>
       </c>
@@ -1137,7 +1139,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="9" t="s">
         <v>15</v>
       </c>
@@ -1147,7 +1149,7 @@
       <c r="F11" s="15"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="18" t="s">
         <v>16</v>
       </c>
@@ -1163,7 +1165,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="18" t="s">
         <v>17</v>
       </c>
@@ -1174,10 +1176,12 @@
       <c r="E13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="12"/>
+      <c r="F13" s="12" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="30"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="19" t="s">
         <v>18</v>
       </c>
@@ -1188,12 +1192,12 @@
         <v>32</v>
       </c>
       <c r="E14" s="7"/>
-      <c r="F14" s="38" t="s">
-        <v>51</v>
+      <c r="F14" s="27" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28">
+      <c r="A15" s="29">
         <v>3</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -1209,7 +1213,7 @@
       <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="18" t="s">
         <v>20</v>
       </c>
@@ -1221,11 +1225,11 @@
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="30"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="19" t="s">
         <v>21</v>
       </c>
@@ -1239,7 +1243,7 @@
       <c r="F17" s="13"/>
     </row>
     <row r="18" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28">
+      <c r="A18" s="29">
         <v>4</v>
       </c>
       <c r="B18" s="26" t="s">
@@ -1251,7 +1255,7 @@
       <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="18" t="s">
         <v>23</v>
       </c>
@@ -1265,7 +1269,7 @@
       <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="18" t="s">
         <v>36</v>
       </c>
@@ -1279,7 +1283,7 @@
       <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="18" t="s">
         <v>24</v>
       </c>
@@ -1293,7 +1297,7 @@
       <c r="F21" s="12"/>
     </row>
     <row r="22" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="30"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="19" t="s">
         <v>25</v>
       </c>
@@ -1304,7 +1308,9 @@
         <v>32</v>
       </c>
       <c r="E22" s="7"/>
-      <c r="F22" s="13"/>
+      <c r="F22" s="13" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23">

</xml_diff>